<commit_message>
First complete implementation for classes
</commit_message>
<xml_diff>
--- a/config/journal.xlsx
+++ b/config/journal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schir\OneDrive\Studium\34_Github\PyPowerSim\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D5A71F-13EA-4AA4-90CC-0446E83FC5AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0567261-BC65-4AF6-8E07-2DF890D750FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="0" windowWidth="9600" windowHeight="10200" activeTab="4" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -1713,7 +1713,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1774,7 +1774,7 @@
         <v>38</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>28</v>
+        <v>114</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>23</v>
@@ -2240,7 +2240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799FBFCB-8244-4B83-8CC9-EBD2890613E5}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -2427,7 +2427,7 @@
         <v>109</v>
       </c>
       <c r="E11" s="13">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>24</v>
@@ -2443,7 +2443,7 @@
         <v>110</v>
       </c>
       <c r="E12" s="13">
-        <v>2.5000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>121</v>
@@ -2537,8 +2537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245B3F0A-B85A-4162-A12D-AC7176B54015}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3200,7 +3200,7 @@
         <v>161</v>
       </c>
       <c r="E33" s="30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F33" s="19" t="s">
         <v>23</v>

</xml_diff>